<commit_message>
Added connection with Excel Sheet
</commit_message>
<xml_diff>
--- a/Book_of_Life.xlsx
+++ b/Book_of_Life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishvik\Desktop\RoutineNet\RouteNet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E8BA262A-ABA1-4F38-A218-E53E0984E61C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CAE8832A-1563-4F75-9C96-C4D8034BC028}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="3" xr2:uid="{958AD86A-C806-446E-93BD-073E4C3CF93E}"/>
   </bookViews>
@@ -57,7 +57,7 @@
     <t>Hour\Emotion</t>
   </si>
   <si>
-    <t>Sleepy</t>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1552C10C-7D79-4950-A2A5-D8189AAA0F6F}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -570,7 +572,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989AA75B-D78D-4095-87D7-FAC04EB19D9B}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -764,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA1D4E9-A0E5-4E18-8AAE-5F671B64C63A}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1039,7 +1043,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1060,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1068,7 +1072,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1076,7 +1080,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.9</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1084,7 +1088,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.9</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1092,7 +1096,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.9</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1100,7 +1104,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.9</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1108,7 +1112,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.9</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1116,7 +1120,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.7</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1124,7 +1128,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1132,7 +1136,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -1140,7 +1144,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -1148,7 +1152,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -1156,7 +1160,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -1164,7 +1168,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -1172,7 +1176,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1180,7 +1184,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1188,7 +1192,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -1196,7 +1200,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1204,7 +1208,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -1212,7 +1216,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -1220,7 +1224,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1228,7 +1232,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.7</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1236,7 +1240,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.9</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>